<commit_message>
Reworked libraries and functions to work
Needed to take the adjustments out of the SSS class to pass functional
tests.
</commit_message>
<xml_diff>
--- a/Datasheet/PinMappingTable.xlsx
+++ b/Datasheet/PinMappingTable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy-daily.UTULSA\Dropbox (JHSI)\Synercon Engineering Documents\SSS\Arduino\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy-daily.UTULSA\Documents\GitHub\SmartSensorSimulator\Datasheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1439,8 +1439,8 @@
   </sheetPr>
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revert "Reworked libraries and functions to work"
This reverts commit 0fdd2c30cdc2ebab1bcddc6791c1e7ffea6b5b89.

Conflicts:
	Arduino Sketch Library/SSS_ADEM4_Rev10_Mega/SSS_ADEM4_Rev10_Mega.ino
	Arduino Sketch Library/libraries/SSS/SSS.cpp
	Arduino Sketch Library/libraries/SSS/SSS.h
</commit_message>
<xml_diff>
--- a/Datasheet/PinMappingTable.xlsx
+++ b/Datasheet/PinMappingTable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy-daily.UTULSA\Documents\GitHub\SmartSensorSimulator\Datasheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy-daily.UTULSA\Dropbox (JHSI)\Synercon Engineering Documents\SSS\Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1439,8 +1439,8 @@
   </sheetPr>
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Production ready libraries for the SSS Rev 10
Libraries are verified for the ATmega2560. Example settings are for the
CAT ADEM4. Updated pin descriptions also.
</commit_message>
<xml_diff>
--- a/Datasheet/PinMappingTable.xlsx
+++ b/Datasheet/PinMappingTable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy-daily.UTULSA\Dropbox (JHSI)\Synercon Engineering Documents\SSS\Arduino\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeremy-daily.UTULSA\Documents\GitHub\SmartSensorSimulator\Datasheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="342">
   <si>
     <t>Pin Number</t>
   </si>
@@ -1032,6 +1032,21 @@
   </si>
   <si>
     <t>Coil 5 Control</t>
+  </si>
+  <si>
+    <t>Main Port Name (Rev 10)</t>
+  </si>
+  <si>
+    <t>LIN CS 5V</t>
+  </si>
+  <si>
+    <t>LIN !Wake 5V</t>
+  </si>
+  <si>
+    <t>LIN RX</t>
+  </si>
+  <si>
+    <t>LIN TX</t>
   </si>
 </sst>
 </file>
@@ -1437,10 +1452,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H102"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,9 +1468,10 @@
     <col min="6" max="6" width="24.28515625" customWidth="1"/>
     <col min="7" max="7" width="24.85546875" style="4" customWidth="1"/>
     <col min="8" max="8" width="21.7109375" customWidth="1"/>
+    <col min="9" max="9" width="24.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>241</v>
       </c>
@@ -1464,7 +1480,7 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1489,8 +1505,11 @@
       <c r="H2" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1515,8 +1534,11 @@
       <c r="H3" s="5" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1543,8 +1565,12 @@
         <f>G4</f>
         <v>IO0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="1" t="str">
+        <f>H4</f>
+        <v>IO0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1564,15 +1590,19 @@
         <v>188</v>
       </c>
       <c r="G5" s="1" t="str">
-        <f t="shared" ref="G5:H6" si="0">F5</f>
+        <f t="shared" ref="G5:I6" si="0">F5</f>
         <v>IO1</v>
       </c>
       <c r="H5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>IO1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>IO1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1597,8 +1627,11 @@
         <f t="shared" si="0"/>
         <v>IO2</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1623,8 +1656,11 @@
       <c r="H7" s="5" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1650,8 +1686,12 @@
       <c r="H8" s="1" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="1" t="str">
+        <f>H8</f>
+        <v>CAN-INT</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1677,8 +1717,11 @@
       <c r="H9" s="1" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1702,8 +1745,11 @@
       <c r="H10" s="1" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1721,15 +1767,19 @@
         <v>195</v>
       </c>
       <c r="G11" s="1" t="str">
-        <f t="shared" ref="G11:H24" si="1">F11</f>
+        <f t="shared" ref="G11:I24" si="1">F11</f>
         <v>Clock</v>
       </c>
       <c r="H11" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Clock</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Clock</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1754,8 +1804,12 @@
         <f t="shared" si="1"/>
         <v>VCC</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>VCC</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1780,8 +1834,12 @@
         <f t="shared" si="1"/>
         <v>GND</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>GND</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1807,8 +1865,11 @@
       <c r="H14" s="1" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1834,8 +1895,11 @@
       <c r="H15" s="1" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1859,8 +1923,11 @@
       <c r="H16" s="1" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1886,8 +1953,11 @@
       <c r="H17" s="1" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1913,8 +1983,11 @@
       <c r="H18" s="1" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1940,8 +2013,11 @@
       <c r="H19" s="1" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1967,8 +2043,11 @@
       <c r="H20" s="1" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1994,8 +2073,11 @@
       <c r="H21" s="1" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2022,8 +2104,11 @@
         <f t="shared" si="1"/>
         <v>SCK</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2050,8 +2135,11 @@
         <f t="shared" si="1"/>
         <v>SDI</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2078,8 +2166,11 @@
         <f t="shared" si="1"/>
         <v>SDO</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2104,8 +2195,11 @@
       <c r="H25" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2130,8 +2224,11 @@
       <c r="H26" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2156,8 +2253,11 @@
       <c r="H27" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2182,8 +2282,11 @@
       <c r="H28" s="1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2207,8 +2310,11 @@
       <c r="H29" s="1" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="1" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2231,8 +2337,11 @@
       <c r="H30" s="1" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2255,8 +2364,11 @@
       <c r="H31" s="1" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2281,8 +2393,12 @@
         <f>G32</f>
         <v>!Reset</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="1" t="str">
+        <f>H32</f>
+        <v>!Reset</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2298,15 +2414,19 @@
         <v>18</v>
       </c>
       <c r="G33" s="1" t="str">
-        <f t="shared" ref="G33:H52" si="2">F33</f>
+        <f t="shared" ref="G33:I52" si="2">F33</f>
         <v>VCC</v>
       </c>
       <c r="H33" s="1" t="str">
         <f t="shared" si="2"/>
         <v>VCC</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>VCC</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2329,8 +2449,12 @@
         <f t="shared" si="2"/>
         <v>GND</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>GND</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2355,8 +2479,12 @@
         <f t="shared" si="2"/>
         <v>XTAL2</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>XTAL2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2381,8 +2509,12 @@
         <f t="shared" si="2"/>
         <v>XTAL1</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>XTAL1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2409,8 +2541,12 @@
         <f t="shared" si="2"/>
         <v>VccSelectU4_0</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>VccSelectU4_0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2437,8 +2573,12 @@
         <f t="shared" si="2"/>
         <v>VccSelectU4_1</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>VccSelectU4_1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2465,8 +2605,12 @@
         <f t="shared" si="2"/>
         <v>VccSelectU4_2</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>VccSelectU4_2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2493,8 +2637,12 @@
         <f t="shared" si="2"/>
         <v>VccSelectU4_3</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>VccSelectU4_3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2521,8 +2669,12 @@
         <f t="shared" si="2"/>
         <v>GroundSelectU4_0</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>GroundSelectU4_0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2549,8 +2701,12 @@
         <f t="shared" si="2"/>
         <v>GroundSelectU4_1</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>GroundSelectU4_1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2577,8 +2733,12 @@
         <f t="shared" si="2"/>
         <v>GroundSelectU4_2</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>GroundSelectU4_2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2605,8 +2765,12 @@
         <f t="shared" si="2"/>
         <v>GroundSelectU4_3</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>GroundSelectU4_3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2633,8 +2797,12 @@
         <f t="shared" si="2"/>
         <v>SCL</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>SCL</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2661,8 +2829,12 @@
         <f t="shared" si="2"/>
         <v>SDA</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>SDA</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2688,8 +2860,11 @@
       <c r="H47" s="1" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2715,8 +2890,11 @@
       <c r="H48" s="1" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2741,8 +2919,12 @@
         <f t="shared" si="2"/>
         <v>!CS-U1</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>!CS-U1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2767,8 +2949,12 @@
         <f t="shared" si="2"/>
         <v>!CS-U2</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>!CS-U2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2793,8 +2979,12 @@
         <f t="shared" si="2"/>
         <v>!CS-U3</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>!CS-U3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2818,8 +3008,12 @@
         <f t="shared" si="2"/>
         <v>!CS-U4</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>!CS-U4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2844,8 +3038,11 @@
       <c r="H53" s="1" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" s="1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2870,8 +3067,11 @@
       <c r="H54" s="1" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" s="1" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2898,8 +3098,12 @@
         <f>G55</f>
         <v>VccSelectU3-0</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" s="1" t="str">
+        <f>H55</f>
+        <v>VccSelectU3-0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2919,15 +3123,19 @@
         <v>264</v>
       </c>
       <c r="G56" s="1" t="str">
-        <f t="shared" ref="G56:H71" si="3">F56</f>
+        <f t="shared" ref="G56:I71" si="3">F56</f>
         <v>VccSelectU3-1</v>
       </c>
       <c r="H56" s="1" t="str">
         <f t="shared" si="3"/>
         <v>VccSelectU3-1</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>VccSelectU3-1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2954,8 +3162,12 @@
         <f t="shared" si="3"/>
         <v>VccSelectU3-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>VccSelectU3-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2982,8 +3194,12 @@
         <f t="shared" si="3"/>
         <v>VccSelectU3-3</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>VccSelectU3-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -3010,8 +3226,12 @@
         <f t="shared" si="3"/>
         <v>GroundSelectU3-0</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>GroundSelectU3-0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -3038,8 +3258,12 @@
         <f t="shared" si="3"/>
         <v>GroundSelectU3-1</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>GroundSelectU3-1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -3066,8 +3290,12 @@
         <f t="shared" si="3"/>
         <v>GroundSelectU3-2</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>GroundSelectU3-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -3094,8 +3322,12 @@
         <f t="shared" si="3"/>
         <v>GroundSelectU3-3</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>GroundSelectU3-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -3118,8 +3350,12 @@
         <f t="shared" si="3"/>
         <v>VCC</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>VCC</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -3142,8 +3378,12 @@
         <f t="shared" si="3"/>
         <v>GND</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>GND</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -3170,8 +3410,12 @@
         <f t="shared" si="3"/>
         <v>VccSelectU2_0</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>VccSelectU2_0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -3198,8 +3442,12 @@
         <f t="shared" si="3"/>
         <v>VccSelectU2_1</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>VccSelectU2_1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -3224,8 +3472,12 @@
         <f t="shared" si="3"/>
         <v>VccSelectU2_2</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>VccSelectU2_2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -3250,8 +3502,12 @@
         <f t="shared" si="3"/>
         <v>VccSelectU2_3</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>VccSelectU2_3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -3276,8 +3532,12 @@
         <f t="shared" si="3"/>
         <v>GroundSelectU2_0</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>GroundSelectU2_0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -3302,8 +3562,12 @@
         <f t="shared" si="3"/>
         <v>GroundSelectU2_1</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>GroundSelectU2_1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -3328,8 +3592,12 @@
         <f t="shared" si="3"/>
         <v>GroundSelectU2_2</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>GroundSelectU2_2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -3354,8 +3622,11 @@
       <c r="H72" s="5" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -3382,8 +3653,12 @@
         <f>G73</f>
         <v>GroundSelectU1_3</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" s="1" t="str">
+        <f>H73</f>
+        <v>GroundSelectU1_3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -3403,15 +3678,19 @@
         <v>223</v>
       </c>
       <c r="G74" s="1" t="str">
-        <f t="shared" ref="G74:H80" si="4">F74</f>
+        <f t="shared" ref="G74:I80" si="4">F74</f>
         <v>GroundSelectU1_2</v>
       </c>
       <c r="H74" s="1" t="str">
         <f t="shared" si="4"/>
         <v>GroundSelectU1_2</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>GroundSelectU1_2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -3438,8 +3717,12 @@
         <f t="shared" si="4"/>
         <v>GroundSelectU1_1</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>GroundSelectU1_1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -3466,8 +3749,12 @@
         <f t="shared" si="4"/>
         <v>GroundSelectU1_0</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>GroundSelectU1_0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -3494,8 +3781,12 @@
         <f t="shared" si="4"/>
         <v>VccSelectU1_3</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>VccSelectU1_3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -3522,8 +3813,12 @@
         <f t="shared" si="4"/>
         <v>VccSelectU1_2</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>VccSelectU1_2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -3550,8 +3845,12 @@
         <f t="shared" si="4"/>
         <v>VccSelectU1_1</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>VccSelectU1_1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -3578,8 +3877,12 @@
         <f t="shared" si="4"/>
         <v>VccSelectU1_0</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>VccSelectU1_0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -3604,8 +3907,12 @@
         <f>G81</f>
         <v>GroundSelectU2_3</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" s="1" t="str">
+        <f>H81</f>
+        <v>GroundSelectU2_3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -3628,8 +3935,12 @@
         <f>G82</f>
         <v>VCC</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82" s="1" t="str">
+        <f>H82</f>
+        <v>VCC</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -3645,15 +3956,19 @@
         <v>19</v>
       </c>
       <c r="G83" s="1" t="str">
-        <f t="shared" ref="G83:H83" si="5">F83</f>
+        <f t="shared" ref="G83:I83" si="5">F83</f>
         <v>GND</v>
       </c>
       <c r="H83" s="1" t="str">
         <f t="shared" si="5"/>
         <v>GND</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>GND</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -3678,8 +3993,11 @@
       <c r="H84" s="1" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -3704,8 +4022,11 @@
       <c r="H85" s="1" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -3730,8 +4051,11 @@
       <c r="H86" s="1" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -3756,8 +4080,11 @@
       <c r="H87" s="1" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -3782,8 +4109,11 @@
       <c r="H88" s="1" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -3808,8 +4138,11 @@
       <c r="H89" s="1" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -3834,8 +4167,11 @@
       <c r="H90" s="1" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -3860,8 +4196,11 @@
       <c r="H91" s="1" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" s="1" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -3886,8 +4225,11 @@
       <c r="H92" s="1" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -3912,8 +4254,11 @@
       <c r="H93" s="1" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -3938,8 +4283,11 @@
       <c r="H94" s="1" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -3964,8 +4312,11 @@
       <c r="H95" s="1" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -3990,8 +4341,11 @@
       <c r="H96" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I96" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -4016,8 +4370,11 @@
       <c r="H97" s="1" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I97" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -4042,8 +4399,11 @@
       <c r="H98" s="1" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -4068,8 +4428,11 @@
       <c r="H99" s="1" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I99" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -4088,8 +4451,11 @@
       <c r="H100" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I100" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -4108,8 +4474,11 @@
       <c r="H101" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I101" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -4126,6 +4495,9 @@
         <v>166</v>
       </c>
       <c r="H102" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I102" s="1" t="s">
         <v>166</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added SSS Daughterboard library.
Fault Free on Exemplar DDEC10.
TODO: Complete mapping out the pins and values for DDEC10.
</commit_message>
<xml_diff>
--- a/Datasheet/PinMappingTable.xlsx
+++ b/Datasheet/PinMappingTable.xlsx
@@ -1125,7 +1125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1139,11 +1139,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1455,7 +1464,7 @@
   <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,21 +1473,21 @@
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
     <col min="4" max="4" width="19.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="4" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" style="4" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="21.7109375" customWidth="1"/>
     <col min="9" max="9" width="24.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1511,924 +1520,901 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="C3" s="3"/>
       <c r="D3" s="1">
-        <v>4</v>
+        <v>81</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>338</v>
+        <v>169</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="G3" s="1" t="str">
+        <f>F3</f>
+        <v>!CS-U1</v>
+      </c>
+      <c r="H3" s="8" t="str">
+        <f>G3</f>
+        <v>!CS-U1</v>
+      </c>
+      <c r="I3" s="1" t="str">
+        <f>H3</f>
+        <v>!CS-U1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="1">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G4" s="1" t="str">
         <f>F4</f>
-        <v>IO0</v>
+        <v>!CS-U2</v>
       </c>
       <c r="H4" s="1" t="str">
         <f>G4</f>
-        <v>IO0</v>
+        <v>!CS-U2</v>
       </c>
       <c r="I4" s="1" t="str">
         <f>H4</f>
-        <v>IO0</v>
+        <v>!CS-U2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C5" s="3"/>
       <c r="D5" s="1">
-        <v>1</v>
+        <v>83</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="G5" s="1" t="str">
-        <f t="shared" ref="G5:I6" si="0">F5</f>
-        <v>IO1</v>
+        <f>F5</f>
+        <v>!CS-U3</v>
       </c>
       <c r="H5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>IO1</v>
+        <f>G5</f>
+        <v>!CS-U3</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>IO1</v>
+        <f>H5</f>
+        <v>!CS-U3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="3"/>
+        <v>82</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="D6" s="1">
-        <v>76</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>189</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E6" s="6"/>
       <c r="F6" s="1" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="G6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>IO2</v>
+        <f>F6</f>
+        <v>!CS-U4</v>
       </c>
       <c r="H6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>IO2</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>327</v>
+        <f>G6</f>
+        <v>!CS-U4</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f>H6</f>
+        <v>!CS-U4</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C7" s="3"/>
       <c r="D7" s="1">
-        <v>5</v>
+        <v>80</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>317</v>
+        <v>255</v>
+      </c>
+      <c r="G7" s="1" t="str">
+        <f>F7</f>
+        <v>D80</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>298</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="G8" s="1" t="str">
-        <f>F8</f>
-        <v>CAN-INT1</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="I8" s="1" t="str">
-        <f>H8</f>
-        <v>CAN-INT</v>
+        <v>252</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="1">
-        <v>3</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="G9" s="1" t="str">
         <f>F9</f>
-        <v>CAN-INT3</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>247</v>
+        <v>!Reset</v>
+      </c>
+      <c r="H9" s="1" t="str">
+        <f>G9</f>
+        <v>!Reset</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f>H9</f>
+        <v>!Reset</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="3"/>
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D10" s="1">
-        <v>77</v>
+        <v>3</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>194</v>
+        <v>247</v>
       </c>
       <c r="G10" s="1" t="str">
         <f>F10</f>
-        <v>IgnitionSelect</v>
+        <v>CAN-INT3</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>194</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>76</v>
+      </c>
       <c r="D11" s="1">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>195</v>
+        <v>261</v>
       </c>
       <c r="G11" s="1" t="str">
-        <f t="shared" ref="G11:I24" si="1">F11</f>
-        <v>Clock</v>
-      </c>
-      <c r="H11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Clock</v>
-      </c>
-      <c r="I11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Clock</v>
+        <f>F11</f>
+        <v>RXD1</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="1">
         <v>18</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>18</v>
+        <v>216</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>18</v>
+        <v>262</v>
       </c>
       <c r="G12" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>VCC</v>
-      </c>
-      <c r="H12" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>VCC</v>
-      </c>
-      <c r="I12" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>VCC</v>
+        <f>F12</f>
+        <v>TXD1</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>19</v>
+        <v>162</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="1"/>
+        <v>163</v>
+      </c>
+      <c r="D13" s="1">
+        <v>54</v>
+      </c>
       <c r="E13" s="1" t="s">
-        <v>19</v>
+        <v>225</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>GND</v>
-      </c>
-      <c r="H13" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>GND</v>
-      </c>
-      <c r="I13" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>GND</v>
+        <v>226</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>96</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>160</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>21</v>
+        <v>161</v>
       </c>
       <c r="D14" s="1">
-        <v>17</v>
+        <v>55</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>186</v>
+        <v>240</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="G14" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>J1708 RX</v>
+        <v>285</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>313</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>320</v>
+        <v>240</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>243</v>
+        <v>313</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>95</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>158</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>23</v>
+        <v>159</v>
       </c>
       <c r="D15" s="1">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>187</v>
+        <v>239</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="G15" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>J1708 TX</v>
+        <v>284</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>312</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>321</v>
+        <v>239</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>244</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="3"/>
+        <v>156</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="D16" s="1">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>180</v>
+        <v>238</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="G16" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>D79</v>
+        <v>283</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>311</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>322</v>
+        <v>238</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>98</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>164</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="1">
-        <v>6</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="G17" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CS-CAN1</v>
+        <v>165</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>323</v>
+        <v>164</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>253</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>166</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="1">
-        <v>7</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="G18" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>CS-CAN3</v>
+        <v>18</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1" t="s">
+        <v>166</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>324</v>
+        <v>166</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>254</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>30</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="C19" s="3"/>
       <c r="D19" s="1">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="G19" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>D8 (PWM1)</v>
+        <v>260</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>290</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>250</v>
+        <v>339</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="G20" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>D9 (PWM2)</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>326</v>
+        <v>190</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>316</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>251</v>
+        <v>338</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D21" s="1">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G21" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>SS</v>
+        <f>F21</f>
+        <v>CAN-INT1</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>248</v>
+        <v>192</v>
+      </c>
+      <c r="I21" s="1" t="str">
+        <f>H21</f>
+        <v>CAN-INT</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>36</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C22" s="3"/>
       <c r="D22" s="1">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G22" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>SCK</v>
+        <f>F22</f>
+        <v>Clock</v>
       </c>
       <c r="H22" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>SCK</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>197</v>
+        <f>G22</f>
+        <v>Clock</v>
+      </c>
+      <c r="I22" s="1" t="str">
+        <f>H22</f>
+        <v>Clock</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>38</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C23" s="3"/>
       <c r="D23" s="1">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G23" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>SDI</v>
-      </c>
-      <c r="H23" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>SDI</v>
+        <v>204</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>327</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>198</v>
+        <v>296</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="1">
         <v>39</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" s="1">
-        <v>50</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="G24" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>SDO</v>
-      </c>
-      <c r="H24" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>SDO</v>
+        <v>190</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>332</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>199</v>
+        <v>299</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="D25" s="1">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>258</v>
+        <v>190</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>200</v>
+        <v>331</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="D26" s="1">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>259</v>
+        <v>190</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>201</v>
+        <v>330</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>45</v>
+        <v>154</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>46</v>
+        <v>155</v>
       </c>
       <c r="D27" s="1">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>202</v>
+        <v>237</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>256</v>
+        <v>282</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>295</v>
+        <v>310</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>202</v>
+        <v>336</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>295</v>
+        <v>310</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>47</v>
+        <v>152</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>48</v>
+        <v>153</v>
       </c>
       <c r="D28" s="1">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>203</v>
+        <v>236</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>257</v>
+        <v>281</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>294</v>
+        <v>309</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>203</v>
+        <v>335</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>294</v>
+        <v>309</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="3"/>
+        <v>150</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>151</v>
+      </c>
       <c r="D29" s="1">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>181</v>
+        <v>235</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="G29" s="1" t="str">
-        <f>F29</f>
-        <v>D80</v>
+        <v>280</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>308</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>298</v>
+        <v>334</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>330</v>
+        <v>308</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="3"/>
+        <v>148</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>149</v>
+      </c>
       <c r="D30" s="1">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>190</v>
+        <v>234</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>204</v>
+        <v>279</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="D31" s="1">
-        <v>85</v>
+        <v>53</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>290</v>
+        <v>248</v>
+      </c>
+      <c r="G31" s="1" t="str">
+        <f>F31</f>
+        <v>SS</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>328</v>
+        <v>196</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>339</v>
+        <v>248</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>204</v>
+        <v>19</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>242</v>
+        <v>19</v>
       </c>
       <c r="G32" s="1" t="str">
         <f>F32</f>
-        <v>!Reset</v>
+        <v>GND</v>
       </c>
       <c r="H32" s="1" t="str">
         <f>G32</f>
-        <v>!Reset</v>
+        <v>GND</v>
       </c>
       <c r="I32" s="1" t="str">
         <f>H32</f>
-        <v>!Reset</v>
+        <v>GND</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G33" s="1" t="str">
-        <f t="shared" ref="G33:I52" si="2">F33</f>
-        <v>VCC</v>
+        <f>F33</f>
+        <v>GND</v>
       </c>
       <c r="H33" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>VCC</v>
+        <f>G33</f>
+        <v>GND</v>
       </c>
       <c r="I33" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>VCC</v>
+        <f>H33</f>
+        <v>GND</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>19</v>
@@ -2442,2066 +2428,2093 @@
         <v>19</v>
       </c>
       <c r="G34" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>F34</f>
         <v>GND</v>
       </c>
       <c r="H34" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>G34</f>
         <v>GND</v>
       </c>
       <c r="I34" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>H34</f>
         <v>GND</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>33</v>
+        <v>81</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="D35" s="1"/>
-      <c r="E35" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="E35" s="1"/>
       <c r="F35" s="1" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="G35" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>XTAL2</v>
+        <f>F35</f>
+        <v>GND</v>
       </c>
       <c r="H35" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>XTAL2</v>
+        <f>G35</f>
+        <v>GND</v>
       </c>
       <c r="I35" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>XTAL2</v>
+        <f>H35</f>
+        <v>GND</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="D36" s="1"/>
-      <c r="E36" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G36" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>XTAL1</v>
-      </c>
-      <c r="H36" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>XTAL1</v>
-      </c>
-      <c r="I36" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>XTAL1</v>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>55</v>
+        <v>121</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>56</v>
+        <v>122</v>
       </c>
       <c r="D37" s="1">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="G37" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>VccSelectU4_0</v>
+        <f>F37</f>
+        <v>GroundSelectU1_0</v>
       </c>
       <c r="H37" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>VccSelectU4_0</v>
+        <f>G37</f>
+        <v>GroundSelectU1_0</v>
       </c>
       <c r="I37" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>VccSelectU4_0</v>
+        <f>H37</f>
+        <v>GroundSelectU1_0</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>58</v>
+        <v>120</v>
       </c>
       <c r="D38" s="1">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>206</v>
+        <v>224</v>
       </c>
       <c r="G38" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>VccSelectU4_1</v>
+        <f>F38</f>
+        <v>GroundSelectU1_1</v>
       </c>
       <c r="H38" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>VccSelectU4_1</v>
+        <f>G38</f>
+        <v>GroundSelectU1_1</v>
       </c>
       <c r="I38" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>VccSelectU4_1</v>
+        <f>H38</f>
+        <v>GroundSelectU1_1</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>59</v>
+        <v>117</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>60</v>
+        <v>118</v>
       </c>
       <c r="D39" s="1">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>207</v>
+        <v>223</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>207</v>
+        <v>223</v>
       </c>
       <c r="G39" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>VccSelectU4_2</v>
+        <f>F39</f>
+        <v>GroundSelectU1_2</v>
       </c>
       <c r="H39" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>VccSelectU4_2</v>
+        <f>G39</f>
+        <v>GroundSelectU1_2</v>
       </c>
       <c r="I39" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>VccSelectU4_2</v>
+        <f>H39</f>
+        <v>GroundSelectU1_2</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>38</v>
+        <v>71</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>61</v>
+        <v>115</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>62</v>
+        <v>116</v>
       </c>
       <c r="D40" s="1">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="G40" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>VccSelectU4_3</v>
+        <f>F40</f>
+        <v>GroundSelectU1_3</v>
       </c>
       <c r="H40" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>VccSelectU4_3</v>
+        <f>G40</f>
+        <v>GroundSelectU1_3</v>
       </c>
       <c r="I40" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>VccSelectU4_3</v>
+        <f>H40</f>
+        <v>GroundSelectU1_3</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>64</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="C41" s="3"/>
       <c r="D41" s="1">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>209</v>
+        <v>176</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>209</v>
+        <v>176</v>
       </c>
       <c r="G41" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>GroundSelectU4_0</v>
+        <f>F41</f>
+        <v>GroundSelectU2_0</v>
       </c>
       <c r="H41" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>GroundSelectU4_0</v>
+        <f>G41</f>
+        <v>GroundSelectU2_0</v>
       </c>
       <c r="I41" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>GroundSelectU4_0</v>
+        <f>H41</f>
+        <v>GroundSelectU2_0</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>66</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="C42" s="3"/>
       <c r="D42" s="1">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>210</v>
+        <v>177</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>210</v>
+        <v>177</v>
       </c>
       <c r="G42" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>GroundSelectU4_1</v>
+        <f>F42</f>
+        <v>GroundSelectU2_1</v>
       </c>
       <c r="H42" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>GroundSelectU4_1</v>
+        <f>G42</f>
+        <v>GroundSelectU2_1</v>
       </c>
       <c r="I42" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>GroundSelectU4_1</v>
+        <f>H42</f>
+        <v>GroundSelectU2_1</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>68</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="C43" s="3"/>
       <c r="D43" s="1">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>211</v>
+        <v>178</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>211</v>
+        <v>178</v>
       </c>
       <c r="G43" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>GroundSelectU4_2</v>
+        <f>F43</f>
+        <v>GroundSelectU2_2</v>
       </c>
       <c r="H43" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>GroundSelectU4_2</v>
+        <f>G43</f>
+        <v>GroundSelectU2_2</v>
       </c>
       <c r="I43" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>GroundSelectU4_2</v>
+        <f>H43</f>
+        <v>GroundSelectU2_2</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="C44" s="3"/>
       <c r="D44" s="1">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>212</v>
+        <v>179</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>212</v>
+        <v>179</v>
       </c>
       <c r="G44" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>GroundSelectU4_3</v>
+        <f>F44</f>
+        <v>GroundSelectU2_3</v>
       </c>
       <c r="H44" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>GroundSelectU4_3</v>
+        <f>G44</f>
+        <v>GroundSelectU2_3</v>
       </c>
       <c r="I44" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>GroundSelectU4_3</v>
+        <f>H44</f>
+        <v>GroundSelectU2_3</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
       <c r="D45" s="1">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>213</v>
+        <v>267</v>
       </c>
       <c r="G45" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>SCL</v>
+        <f>F45</f>
+        <v>GroundSelectU3-0</v>
       </c>
       <c r="H45" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>SCL</v>
+        <f>G45</f>
+        <v>GroundSelectU3-0</v>
       </c>
       <c r="I45" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>SCL</v>
+        <f>H45</f>
+        <v>GroundSelectU3-0</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="D46" s="1">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>214</v>
+        <v>190</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>214</v>
+        <v>268</v>
       </c>
       <c r="G46" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>SDA</v>
+        <f>F46</f>
+        <v>GroundSelectU3-1</v>
       </c>
       <c r="H46" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>SDA</v>
+        <f>G46</f>
+        <v>GroundSelectU3-1</v>
       </c>
       <c r="I46" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>SDA</v>
+        <f>H46</f>
+        <v>GroundSelectU3-1</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
       <c r="D47" s="1">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>215</v>
+        <v>190</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="G47" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>RXD1</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>340</v>
+        <f>F47</f>
+        <v>GroundSelectU3-2</v>
+      </c>
+      <c r="H47" s="1" t="str">
+        <f>G47</f>
+        <v>GroundSelectU3-2</v>
+      </c>
+      <c r="I47" s="1" t="str">
+        <f>H47</f>
+        <v>GroundSelectU3-2</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="D48" s="1">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>262</v>
+        <v>190</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>270</v>
       </c>
       <c r="G48" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>TXD1</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>341</v>
+        <f>F48</f>
+        <v>GroundSelectU3-3</v>
+      </c>
+      <c r="H48" s="1" t="str">
+        <f>G48</f>
+        <v>GroundSelectU3-3</v>
+      </c>
+      <c r="I48" s="1" t="str">
+        <f>H48</f>
+        <v>GroundSelectU3-3</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C49" s="3"/>
+        <v>63</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="D49" s="1">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>169</v>
+        <v>209</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="G49" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>!CS-U1</v>
+        <f>F49</f>
+        <v>GroundSelectU4_0</v>
       </c>
       <c r="H49" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>!CS-U1</v>
+        <f>G49</f>
+        <v>GroundSelectU4_0</v>
       </c>
       <c r="I49" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>!CS-U1</v>
+        <f>H49</f>
+        <v>GroundSelectU4_0</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C50" s="3"/>
+        <v>65</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="D50" s="1">
-        <v>82</v>
+        <v>44</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>170</v>
+        <v>210</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>169</v>
+        <v>210</v>
       </c>
       <c r="G50" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>!CS-U2</v>
+        <f>F50</f>
+        <v>GroundSelectU4_1</v>
       </c>
       <c r="H50" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>!CS-U2</v>
+        <f>G50</f>
+        <v>GroundSelectU4_1</v>
       </c>
       <c r="I50" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>!CS-U2</v>
+        <f>H50</f>
+        <v>GroundSelectU4_1</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C51" s="3"/>
+        <v>67</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="D51" s="1">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>171</v>
+        <v>211</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>170</v>
+        <v>211</v>
       </c>
       <c r="G51" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>!CS-U3</v>
+        <f>F51</f>
+        <v>GroundSelectU4_2</v>
       </c>
       <c r="H51" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>!CS-U3</v>
+        <f>G51</f>
+        <v>GroundSelectU4_2</v>
       </c>
       <c r="I51" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>!CS-U3</v>
+        <f>H51</f>
+        <v>GroundSelectU4_2</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="D52" s="1">
-        <v>38</v>
+        <v>42</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>212</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>171</v>
+        <v>212</v>
       </c>
       <c r="G52" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>!CS-U4</v>
+        <f>F52</f>
+        <v>GroundSelectU4_3</v>
       </c>
       <c r="H52" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>!CS-U4</v>
+        <f>G52</f>
+        <v>GroundSelectU4_3</v>
       </c>
       <c r="I52" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>!CS-U4</v>
+        <f>H52</f>
+        <v>GroundSelectU4_3</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>84</v>
+        <v>140</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>85</v>
+        <v>141</v>
       </c>
       <c r="D53" s="1">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>190</v>
+        <v>230</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>190</v>
+        <v>275</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>330</v>
+        <v>302</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>52</v>
+        <v>87</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>86</v>
+        <v>142</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>87</v>
+        <v>143</v>
       </c>
       <c r="D54" s="1">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>190</v>
+        <v>276</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>331</v>
+        <v>301</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>88</v>
+        <v>144</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>89</v>
+        <v>145</v>
       </c>
       <c r="D55" s="1">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>190</v>
+        <v>232</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="G55" s="1" t="str">
-        <f>F55</f>
-        <v>VccSelectU3-0</v>
-      </c>
-      <c r="H55" s="1" t="str">
-        <f>G55</f>
-        <v>VccSelectU3-0</v>
-      </c>
-      <c r="I55" s="1" t="str">
-        <f>H55</f>
-        <v>VccSelectU3-0</v>
+        <v>277</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>90</v>
+        <v>146</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>91</v>
+        <v>147</v>
       </c>
       <c r="D56" s="1">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>190</v>
+        <v>233</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="G56" s="1" t="str">
-        <f t="shared" ref="G56:I71" si="3">F56</f>
-        <v>VccSelectU3-1</v>
-      </c>
-      <c r="H56" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VccSelectU3-1</v>
-      </c>
-      <c r="I56" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VccSelectU3-1</v>
+        <v>278</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>92</v>
+        <v>5</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>93</v>
+        <v>6</v>
       </c>
       <c r="D57" s="1">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>265</v>
+        <v>168</v>
       </c>
       <c r="G57" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VccSelectU3-2</v>
+        <f>F57</f>
+        <v>IO0</v>
       </c>
       <c r="H57" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VccSelectU3-2</v>
+        <f>G57</f>
+        <v>IO0</v>
       </c>
       <c r="I57" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VccSelectU3-2</v>
+        <f>H57</f>
+        <v>IO0</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>95</v>
+        <v>8</v>
       </c>
       <c r="D58" s="1">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>266</v>
+        <v>188</v>
       </c>
       <c r="G58" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VccSelectU3-3</v>
+        <f>F58</f>
+        <v>IO1</v>
       </c>
       <c r="H58" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VccSelectU3-3</v>
+        <f>G58</f>
+        <v>IO1</v>
       </c>
       <c r="I58" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VccSelectU3-3</v>
+        <f>H58</f>
+        <v>IO1</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>57</v>
+        <v>4</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>97</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C59" s="3"/>
       <c r="D59" s="1">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>267</v>
+        <v>189</v>
       </c>
       <c r="G59" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU3-0</v>
+        <f>F59</f>
+        <v>IO2</v>
       </c>
       <c r="H59" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU3-0</v>
-      </c>
-      <c r="I59" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU3-0</v>
+        <f>G59</f>
+        <v>IO2</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>99</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C60" s="3"/>
       <c r="D60" s="1">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>268</v>
+        <v>245</v>
       </c>
       <c r="G60" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU3-1</v>
-      </c>
-      <c r="H60" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU3-1</v>
-      </c>
-      <c r="I60" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU3-1</v>
+        <f>F60</f>
+        <v>D79</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>101</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C61" s="3"/>
       <c r="D61" s="1">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>269</v>
+        <v>194</v>
       </c>
       <c r="G61" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU3-2</v>
-      </c>
-      <c r="H61" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU3-2</v>
-      </c>
-      <c r="I61" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU3-2</v>
+        <f>F61</f>
+        <v>IgnitionSelect</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>102</v>
+        <v>25</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>103</v>
+        <v>26</v>
       </c>
       <c r="D62" s="1">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>270</v>
+        <v>185</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>253</v>
       </c>
       <c r="G62" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU3-3</v>
-      </c>
-      <c r="H62" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU3-3</v>
-      </c>
-      <c r="I62" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU3-3</v>
+        <f>F62</f>
+        <v>CS-CAN1</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
+        <v>28</v>
+      </c>
+      <c r="D63" s="1">
+        <v>7</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>184</v>
+      </c>
       <c r="F63" s="1" t="s">
-        <v>18</v>
+        <v>254</v>
       </c>
       <c r="G63" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VCC</v>
-      </c>
-      <c r="H63" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VCC</v>
-      </c>
-      <c r="I63" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VCC</v>
+        <f>F63</f>
+        <v>CS-CAN3</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>62</v>
+        <v>17</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="D64" s="1">
+        <v>8</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>183</v>
+      </c>
       <c r="F64" s="1" t="s">
-        <v>19</v>
+        <v>250</v>
       </c>
       <c r="G64" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GND</v>
-      </c>
-      <c r="H64" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GND</v>
-      </c>
-      <c r="I64" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GND</v>
+        <f>F64</f>
+        <v>D8 (PWM1)</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>104</v>
+        <v>31</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="D65" s="1">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>172</v>
+        <v>251</v>
       </c>
       <c r="G65" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VccSelectU2_0</v>
-      </c>
-      <c r="H65" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VccSelectU2_0</v>
-      </c>
-      <c r="I65" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VccSelectU2_0</v>
+        <f>F65</f>
+        <v>D9 (PWM2)</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>106</v>
+        <v>41</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>107</v>
+        <v>42</v>
       </c>
       <c r="D66" s="1">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>173</v>
+        <v>200</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="G66" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VccSelectU2_1</v>
-      </c>
-      <c r="H66" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VccSelectU2_1</v>
-      </c>
-      <c r="I66" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VccSelectU2_1</v>
+        <v>258</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C67" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="D67" s="1">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>174</v>
+        <v>201</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="G67" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VccSelectU2_2</v>
-      </c>
-      <c r="H67" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VccSelectU2_2</v>
-      </c>
-      <c r="I67" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VccSelectU2_2</v>
+        <v>259</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C68" s="3"/>
+        <v>45</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>46</v>
+      </c>
       <c r="D68" s="1">
-        <v>71</v>
+        <v>12</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>175</v>
+        <v>202</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="G68" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VccSelectU2_3</v>
-      </c>
-      <c r="H68" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VccSelectU2_3</v>
-      </c>
-      <c r="I68" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>VccSelectU2_3</v>
+        <v>256</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C69" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>48</v>
+      </c>
       <c r="D69" s="1">
-        <v>72</v>
+        <v>13</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>176</v>
+        <v>203</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="G69" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU2_0</v>
-      </c>
-      <c r="H69" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU2_0</v>
-      </c>
-      <c r="I69" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU2_0</v>
+        <v>257</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C70" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="D70" s="1">
-        <v>73</v>
+        <v>17</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>177</v>
+        <v>243</v>
       </c>
       <c r="G70" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU2_1</v>
-      </c>
-      <c r="H70" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU2_1</v>
-      </c>
-      <c r="I70" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU2_1</v>
+        <f>F70</f>
+        <v>J1708 RX</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C71" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="D71" s="1">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="G71" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU2_2</v>
+        <f>F71</f>
+        <v>SCK</v>
       </c>
       <c r="H71" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU2_2</v>
-      </c>
-      <c r="I71" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>GroundSelectU2_2</v>
+        <f>G71</f>
+        <v>SCK</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>70</v>
+        <v>43</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>113</v>
+        <v>71</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>114</v>
+        <v>72</v>
       </c>
       <c r="D72" s="1">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>190</v>
+        <v>213</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="H72" s="5" t="s">
-        <v>332</v>
-      </c>
-      <c r="I72" s="1" t="s">
-        <v>299</v>
+        <v>213</v>
+      </c>
+      <c r="G72" s="1" t="str">
+        <f>F72</f>
+        <v>SCL</v>
+      </c>
+      <c r="H72" s="8" t="str">
+        <f>G72</f>
+        <v>SCL</v>
+      </c>
+      <c r="I72" s="1" t="str">
+        <f>H72</f>
+        <v>SCL</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>115</v>
+        <v>73</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="D73" s="1">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="G73" s="1" t="str">
         <f>F73</f>
-        <v>GroundSelectU1_3</v>
+        <v>SDA</v>
       </c>
       <c r="H73" s="1" t="str">
         <f>G73</f>
-        <v>GroundSelectU1_3</v>
+        <v>SDA</v>
       </c>
       <c r="I73" s="1" t="str">
         <f>H73</f>
-        <v>GroundSelectU1_3</v>
+        <v>SDA</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>117</v>
+        <v>37</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="D74" s="1">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>223</v>
+        <v>198</v>
       </c>
       <c r="G74" s="1" t="str">
-        <f t="shared" ref="G74:I80" si="4">F74</f>
-        <v>GroundSelectU1_2</v>
+        <f>F74</f>
+        <v>SDI</v>
       </c>
       <c r="H74" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>GroundSelectU1_2</v>
-      </c>
-      <c r="I74" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>GroundSelectU1_2</v>
+        <f>G74</f>
+        <v>SDI</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>119</v>
+        <v>39</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="D75" s="1">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
       <c r="G75" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>GroundSelectU1_1</v>
+        <f>F75</f>
+        <v>SDO</v>
       </c>
       <c r="H75" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>GroundSelectU1_1</v>
-      </c>
-      <c r="I75" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>GroundSelectU1_1</v>
+        <f>G75</f>
+        <v>SDO</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>121</v>
+        <v>22</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>122</v>
+        <v>23</v>
       </c>
       <c r="D76" s="1">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>221</v>
+        <v>187</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>221</v>
+        <v>244</v>
       </c>
       <c r="G76" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>GroundSelectU1_0</v>
-      </c>
-      <c r="H76" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>GroundSelectU1_0</v>
-      </c>
-      <c r="I76" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>GroundSelectU1_0</v>
+        <f>F76</f>
+        <v>J1708 TX</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>75</v>
+        <v>10</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>123</v>
+        <v>18</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D77" s="1">
-        <v>25</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D77" s="1"/>
       <c r="E77" s="1" t="s">
-        <v>218</v>
+        <v>18</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>218</v>
+        <v>18</v>
       </c>
       <c r="G77" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>VccSelectU1_3</v>
+        <f>F77</f>
+        <v>VCC</v>
       </c>
       <c r="H77" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>VccSelectU1_3</v>
+        <f>G77</f>
+        <v>VCC</v>
       </c>
       <c r="I77" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>VccSelectU1_3</v>
+        <f>H77</f>
+        <v>VCC</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>125</v>
+        <v>18</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D78" s="1">
-        <v>24</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>219</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
       <c r="F78" s="1" t="s">
-        <v>219</v>
+        <v>18</v>
       </c>
       <c r="G78" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>VccSelectU1_2</v>
+        <f>F78</f>
+        <v>VCC</v>
       </c>
       <c r="H78" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>VccSelectU1_2</v>
+        <f>G78</f>
+        <v>VCC</v>
       </c>
       <c r="I78" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>VccSelectU1_2</v>
+        <f>H78</f>
+        <v>VCC</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>127</v>
+        <v>18</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D79" s="1">
-        <v>23</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>220</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
-        <v>220</v>
+        <v>18</v>
       </c>
       <c r="G79" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>VccSelectU1_1</v>
+        <f>F79</f>
+        <v>VCC</v>
       </c>
       <c r="H79" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>VccSelectU1_1</v>
+        <f>G79</f>
+        <v>VCC</v>
       </c>
       <c r="I79" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>VccSelectU1_1</v>
+        <f>H79</f>
+        <v>VCC</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>129</v>
+        <v>18</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D80" s="1">
-        <v>22</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>217</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
       <c r="F80" s="1" t="s">
-        <v>217</v>
+        <v>18</v>
       </c>
       <c r="G80" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>VccSelectU1_0</v>
+        <f>F80</f>
+        <v>VCC</v>
       </c>
       <c r="H80" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>VccSelectU1_0</v>
+        <f>G80</f>
+        <v>VCC</v>
       </c>
       <c r="I80" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>VccSelectU1_0</v>
+        <f>H80</f>
+        <v>VCC</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="C81" s="3"/>
+        <v>129</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>130</v>
+      </c>
       <c r="D81" s="1">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>179</v>
+        <v>217</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>179</v>
+        <v>217</v>
       </c>
       <c r="G81" s="1" t="str">
         <f>F81</f>
-        <v>GroundSelectU2_3</v>
+        <v>VccSelectU1_0</v>
       </c>
       <c r="H81" s="1" t="str">
         <f>G81</f>
-        <v>GroundSelectU2_3</v>
+        <v>VccSelectU1_0</v>
       </c>
       <c r="I81" s="1" t="str">
         <f>H81</f>
-        <v>GroundSelectU2_3</v>
+        <v>VccSelectU1_0</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>18</v>
+        <v>127</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
+        <v>128</v>
+      </c>
+      <c r="D82" s="1">
+        <v>23</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>220</v>
+      </c>
       <c r="F82" s="1" t="s">
-        <v>18</v>
+        <v>220</v>
       </c>
       <c r="G82" s="1" t="str">
         <f>F82</f>
-        <v>VCC</v>
+        <v>VccSelectU1_1</v>
       </c>
       <c r="H82" s="1" t="str">
         <f>G82</f>
-        <v>VCC</v>
+        <v>VccSelectU1_1</v>
       </c>
       <c r="I82" s="1" t="str">
         <f>H82</f>
-        <v>VCC</v>
+        <v>VccSelectU1_1</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>19</v>
+        <v>125</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="D83" s="1">
+        <v>24</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>219</v>
+      </c>
       <c r="F83" s="1" t="s">
-        <v>19</v>
+        <v>219</v>
       </c>
       <c r="G83" s="1" t="str">
-        <f t="shared" ref="G83:I83" si="5">F83</f>
-        <v>GND</v>
+        <f>F83</f>
+        <v>VccSelectU1_2</v>
       </c>
       <c r="H83" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>GND</v>
+        <f>G83</f>
+        <v>VccSelectU1_2</v>
       </c>
       <c r="I83" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>GND</v>
+        <f>H83</f>
+        <v>VccSelectU1_2</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="D84" s="1">
-        <v>69</v>
+        <v>25</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="I84" s="1" t="s">
-        <v>226</v>
+        <v>218</v>
+      </c>
+      <c r="G84" s="1" t="str">
+        <f>F84</f>
+        <v>VccSelectU1_3</v>
+      </c>
+      <c r="H84" s="1" t="str">
+        <f>G84</f>
+        <v>VccSelectU1_3</v>
+      </c>
+      <c r="I84" s="1" t="str">
+        <f>H84</f>
+        <v>VccSelectU1_3</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="D85" s="1">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>227</v>
+        <v>172</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="I85" s="1" t="s">
-        <v>300</v>
+        <v>172</v>
+      </c>
+      <c r="G85" s="1" t="str">
+        <f>F85</f>
+        <v>VccSelectU2_0</v>
+      </c>
+      <c r="H85" s="1" t="str">
+        <f>G85</f>
+        <v>VccSelectU2_0</v>
+      </c>
+      <c r="I85" s="1" t="str">
+        <f>H85</f>
+        <v>VccSelectU2_0</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
       <c r="D86" s="1">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>228</v>
+        <v>173</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="G86" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="H86" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="I86" s="1" t="s">
-        <v>301</v>
+        <v>173</v>
+      </c>
+      <c r="G86" s="1" t="str">
+        <f>F86</f>
+        <v>VccSelectU2_1</v>
+      </c>
+      <c r="H86" s="1" t="str">
+        <f>G86</f>
+        <v>VccSelectU2_1</v>
+      </c>
+      <c r="I86" s="1" t="str">
+        <f>H86</f>
+        <v>VccSelectU2_1</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>139</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="C87" s="3"/>
       <c r="D87" s="1">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>229</v>
+        <v>174</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="H87" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="I87" s="1" t="s">
-        <v>302</v>
+        <v>174</v>
+      </c>
+      <c r="G87" s="1" t="str">
+        <f>F87</f>
+        <v>VccSelectU2_2</v>
+      </c>
+      <c r="H87" s="1" t="str">
+        <f>G87</f>
+        <v>VccSelectU2_2</v>
+      </c>
+      <c r="I87" s="1" t="str">
+        <f>H87</f>
+        <v>VccSelectU2_2</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>141</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="C88" s="3"/>
       <c r="D88" s="1">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>230</v>
+        <v>175</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="H88" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="I88" s="1" t="s">
-        <v>303</v>
+        <v>175</v>
+      </c>
+      <c r="G88" s="1" t="str">
+        <f>F88</f>
+        <v>VccSelectU2_3</v>
+      </c>
+      <c r="H88" s="1" t="str">
+        <f>G88</f>
+        <v>VccSelectU2_3</v>
+      </c>
+      <c r="I88" s="1" t="str">
+        <f>H88</f>
+        <v>VccSelectU2_3</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>142</v>
+        <v>88</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>143</v>
+        <v>89</v>
       </c>
       <c r="D89" s="1">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>231</v>
+        <v>190</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>304</v>
-      </c>
-      <c r="H89" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="I89" s="1" t="s">
-        <v>304</v>
+        <v>263</v>
+      </c>
+      <c r="G89" s="1" t="str">
+        <f>F89</f>
+        <v>VccSelectU3-0</v>
+      </c>
+      <c r="H89" s="1" t="str">
+        <f>G89</f>
+        <v>VccSelectU3-0</v>
+      </c>
+      <c r="I89" s="1" t="str">
+        <f>H89</f>
+        <v>VccSelectU3-0</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>144</v>
+        <v>90</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>145</v>
+        <v>91</v>
       </c>
       <c r="D90" s="1">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>232</v>
+        <v>190</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="H90" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="I90" s="1" t="s">
-        <v>305</v>
+        <v>264</v>
+      </c>
+      <c r="G90" s="1" t="str">
+        <f>F90</f>
+        <v>VccSelectU3-1</v>
+      </c>
+      <c r="H90" s="1" t="str">
+        <f>G90</f>
+        <v>VccSelectU3-1</v>
+      </c>
+      <c r="I90" s="1" t="str">
+        <f>H90</f>
+        <v>VccSelectU3-1</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>146</v>
+        <v>92</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>147</v>
+        <v>93</v>
       </c>
       <c r="D91" s="1">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>233</v>
+        <v>190</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="H91" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="I91" s="1" t="s">
-        <v>306</v>
+        <v>265</v>
+      </c>
+      <c r="G91" s="1" t="str">
+        <f>F91</f>
+        <v>VccSelectU3-2</v>
+      </c>
+      <c r="H91" s="1" t="str">
+        <f>G91</f>
+        <v>VccSelectU3-2</v>
+      </c>
+      <c r="I91" s="1" t="str">
+        <f>H91</f>
+        <v>VccSelectU3-2</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>148</v>
+        <v>94</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>149</v>
+        <v>95</v>
       </c>
       <c r="D92" s="1">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>234</v>
+        <v>190</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="H92" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="I92" s="1" t="s">
-        <v>307</v>
+        <v>266</v>
+      </c>
+      <c r="G92" s="1" t="str">
+        <f>F92</f>
+        <v>VccSelectU3-3</v>
+      </c>
+      <c r="H92" s="1" t="str">
+        <f>G92</f>
+        <v>VccSelectU3-3</v>
+      </c>
+      <c r="I92" s="1" t="str">
+        <f>H92</f>
+        <v>VccSelectU3-3</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>150</v>
+        <v>55</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>151</v>
+        <v>56</v>
       </c>
       <c r="D93" s="1">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="H93" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="I93" s="1" t="s">
-        <v>308</v>
+        <v>205</v>
+      </c>
+      <c r="G93" s="1" t="str">
+        <f>F93</f>
+        <v>VccSelectU4_0</v>
+      </c>
+      <c r="H93" s="1" t="str">
+        <f>G93</f>
+        <v>VccSelectU4_0</v>
+      </c>
+      <c r="I93" s="1" t="str">
+        <f>H93</f>
+        <v>VccSelectU4_0</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>92</v>
+        <v>36</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>152</v>
+        <v>57</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>153</v>
+        <v>58</v>
       </c>
       <c r="D94" s="1">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>236</v>
+        <v>206</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="H94" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="I94" s="1" t="s">
-        <v>309</v>
+        <v>206</v>
+      </c>
+      <c r="G94" s="1" t="str">
+        <f>F94</f>
+        <v>VccSelectU4_1</v>
+      </c>
+      <c r="H94" s="1" t="str">
+        <f>G94</f>
+        <v>VccSelectU4_1</v>
+      </c>
+      <c r="I94" s="1" t="str">
+        <f>H94</f>
+        <v>VccSelectU4_1</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>93</v>
+        <v>37</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>154</v>
+        <v>59</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>155</v>
+        <v>60</v>
       </c>
       <c r="D95" s="1">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>237</v>
+        <v>207</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="H95" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="I95" s="1" t="s">
-        <v>310</v>
+        <v>207</v>
+      </c>
+      <c r="G95" s="1" t="str">
+        <f>F95</f>
+        <v>VccSelectU4_2</v>
+      </c>
+      <c r="H95" s="1" t="str">
+        <f>G95</f>
+        <v>VccSelectU4_2</v>
+      </c>
+      <c r="I95" s="1" t="str">
+        <f>H95</f>
+        <v>VccSelectU4_2</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>156</v>
+        <v>61</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>157</v>
+        <v>62</v>
       </c>
       <c r="D96" s="1">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>238</v>
+        <v>208</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="G96" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="H96" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="I96" s="1" t="s">
-        <v>311</v>
+        <v>208</v>
+      </c>
+      <c r="G96" s="1" t="str">
+        <f>F96</f>
+        <v>VccSelectU4_3</v>
+      </c>
+      <c r="H96" s="1" t="str">
+        <f>G96</f>
+        <v>VccSelectU4_3</v>
+      </c>
+      <c r="I96" s="1" t="str">
+        <f>H96</f>
+        <v>VccSelectU4_3</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>159</v>
+        <v>133</v>
       </c>
       <c r="D97" s="1">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>312</v>
+        <v>226</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>239</v>
+        <v>306</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>312</v>
+        <v>226</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>160</v>
+        <v>134</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="D98" s="1">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>240</v>
+        <v>305</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="D99" s="1">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>226</v>
+        <v>273</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>225</v>
+        <v>304</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
-      <c r="F100" s="1"/>
+        <v>139</v>
+      </c>
+      <c r="D100" s="1">
+        <v>66</v>
+      </c>
+      <c r="E100" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>274</v>
+      </c>
       <c r="G100" s="1" t="s">
-        <v>164</v>
+        <v>302</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>164</v>
+        <v>303</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>164</v>
+        <v>302</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>99</v>
+        <v>34</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
       <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
-      <c r="F101" s="1"/>
-      <c r="G101" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H101" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I101" s="1" t="s">
-        <v>19</v>
+      <c r="E101" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G101" s="1" t="str">
+        <f>F101</f>
+        <v>XTAL1</v>
+      </c>
+      <c r="H101" s="1" t="str">
+        <f>G101</f>
+        <v>XTAL1</v>
+      </c>
+      <c r="I101" s="1" t="str">
+        <f>H101</f>
+        <v>XTAL1</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>166</v>
+        <v>53</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="D102" s="1"/>
-      <c r="E102" s="1"/>
-      <c r="F102" s="1"/>
-      <c r="G102" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="H102" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="I102" s="1" t="s">
-        <v>166</v>
+      <c r="E102" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G102" s="1" t="str">
+        <f>F102</f>
+        <v>XTAL2</v>
+      </c>
+      <c r="H102" s="1" t="str">
+        <f>G102</f>
+        <v>XTAL2</v>
+      </c>
+      <c r="I102" s="1" t="str">
+        <f>H102</f>
+        <v>XTAL2</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A3:I102">
+    <sortCondition ref="H3"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>

</xml_diff>